<commit_message>
Add total number of customers per continent table to customer_locations sheet
</commit_message>
<xml_diff>
--- a/northwind_business_analysis.xlsx
+++ b/northwind_business_analysis.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/valeriemagalong/Documents/Bootcamp Applications &amp; Prep/Personal Projects/Northwind_Business_Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6C872664-F7C6-AD47-B5C6-FC425811393C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5943FBE5-E04A-3747-A3CF-4E66D269E349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39720" yWindow="2700" windowWidth="28040" windowHeight="17440" xr2:uid="{6C0EAFC1-5571-664F-BC5B-EF13F60EAA6F}"/>
+    <workbookView xWindow="40520" yWindow="500" windowWidth="28040" windowHeight="21080" xr2:uid="{6C0EAFC1-5571-664F-BC5B-EF13F60EAA6F}"/>
   </bookViews>
   <sheets>
-    <sheet name="customer_countries" sheetId="1" r:id="rId1"/>
+    <sheet name="customer_locations" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="27">
   <si>
     <t>Argentina</t>
   </si>
@@ -114,6 +114,9 @@
   </si>
   <si>
     <t>North America</t>
+  </si>
+  <si>
+    <t>Total Number of Customers</t>
   </si>
 </sst>
 </file>
@@ -145,7 +148,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -153,13 +156,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -474,188 +493,212 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE16AF52-CC2D-3443-87C4-0D198942EBDD}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="161" zoomScaleNormal="161" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="D1" s="2"/>
+      <c r="E1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="B4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="B5" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="B6" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="B7" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="B8" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="B9" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="B10" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="B11" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="B12" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B13" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="B13" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B14" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="B14" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B15" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="B15" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="A17" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="A18" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="A19" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="A20" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="A21" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="2" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>